<commit_message>
update sulle tabelle ma resta il problema su update dei files
</commit_message>
<xml_diff>
--- a/files/Benpoker.xlsx
+++ b/files/Benpoker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtaur\Documents\streamlit\apps\hellow\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtaur\Documents\streamlit\apps\benpoker\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224853FC-DC28-4657-AA1D-7AE8F622FF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE55BA2-4B2C-488D-9CD1-BCCB09773082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{5C3A4B80-7231-4572-AA94-9A9D5BEEACD8}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>MasterLeague</t>
   </si>
   <si>
-    <t>Vittorie</t>
-  </si>
-  <si>
     <t>PG</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Tot Cash Vinto</t>
+  </si>
+  <si>
+    <t>Podi</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
     <tableColumn id="17" xr3:uid="{3E44300B-2868-4698-92E9-DBC70914C594}" uniqueName="17" name="Sconfitte" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{46115588-60F0-4C19-9B33-B14993EECEA2}" uniqueName="18" name="PG" queryTableFieldId="18"/>
     <tableColumn id="19" xr3:uid="{451C1AC6-33F2-4B3C-BD62-92D619F74267}" uniqueName="19" name="Tot Cash Vinto" queryTableFieldId="19"/>
-    <tableColumn id="20" xr3:uid="{5937F88E-52BA-478C-86E6-3AC20B16CDB2}" uniqueName="20" name="Vittorie" queryTableFieldId="20"/>
+    <tableColumn id="20" xr3:uid="{5937F88E-52BA-478C-86E6-3AC20B16CDB2}" uniqueName="20" name="Podi" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{3C1DC550-FA23-4D39-BD03-48107936EA4F}" uniqueName="21" name="MasterLeague" queryTableFieldId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -520,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79258609-E536-4A21-AB16-7120817ACE65}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,22 +539,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>14</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -905,8 +905,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="M21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correzioni su nomi e foto
</commit_message>
<xml_diff>
--- a/files/Benpoker.xlsx
+++ b/files/Benpoker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtaur\Documents\streamlit\apps\benpoker\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CADAEF8-F995-4104-A093-F1550198D42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA8618C-2240-4799-B376-BE9AD8310735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="504" windowWidth="23040" windowHeight="12120" xr2:uid="{5C3A4B80-7231-4572-AA94-9A9D5BEEACD8}"/>
+    <workbookView xWindow="2472" yWindow="1020" windowWidth="23040" windowHeight="12120" xr2:uid="{5C3A4B80-7231-4572-AA94-9A9D5BEEACD8}"/>
   </bookViews>
   <sheets>
     <sheet name="classifiche" sheetId="3" r:id="rId1"/>
@@ -41,48 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>domtheboneless</t>
-  </si>
-  <si>
-    <t>sgenchi</t>
-  </si>
-  <si>
-    <t>wawwo</t>
-  </si>
-  <si>
-    <t>Bambarlo</t>
-  </si>
-  <si>
-    <t>Luca</t>
-  </si>
-  <si>
-    <t>Marco</t>
-  </si>
-  <si>
-    <t>Piero</t>
-  </si>
-  <si>
-    <t>Rastroni</t>
-  </si>
-  <si>
-    <t>binzio</t>
-  </si>
-  <si>
-    <t>cman</t>
-  </si>
-  <si>
-    <t>saddave</t>
-  </si>
-  <si>
-    <t>toto007</t>
-  </si>
-  <si>
-    <t>lilith</t>
-  </si>
-  <si>
-    <t>spada</t>
-  </si>
-  <si>
     <t>MasterLeague</t>
   </si>
   <si>
@@ -95,9 +53,6 @@
     <t>Punti</t>
   </si>
   <si>
-    <t>Sanzione</t>
-  </si>
-  <si>
     <t>Giocatore</t>
   </si>
   <si>
@@ -105,6 +60,51 @@
   </si>
   <si>
     <t>Podi</t>
+  </si>
+  <si>
+    <t>Giancarlo Tauro</t>
+  </si>
+  <si>
+    <t>Fabrizio Fresa</t>
+  </si>
+  <si>
+    <t>Nicola Cuomo</t>
+  </si>
+  <si>
+    <t>Domenico Carella</t>
+  </si>
+  <si>
+    <t>Luca De Tommasi</t>
+  </si>
+  <si>
+    <t>Marco Insabato</t>
+  </si>
+  <si>
+    <t>Piero Falagario</t>
+  </si>
+  <si>
+    <t>Antonio Rafaschieri</t>
+  </si>
+  <si>
+    <t>Dave Colaianni</t>
+  </si>
+  <si>
+    <t>Antonio Sanzone</t>
+  </si>
+  <si>
+    <t>Silvio Genchi</t>
+  </si>
+  <si>
+    <t>Giulia Spadafina</t>
+  </si>
+  <si>
+    <t>Giuseppe Toto</t>
+  </si>
+  <si>
+    <t>Walter Spadafina</t>
+  </si>
+  <si>
+    <t>Lilly Antonacci</t>
   </si>
 </sst>
 </file>
@@ -523,12 +523,12 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
@@ -539,68 +539,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>11</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -608,30 +608,30 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>49</v>
@@ -654,22 +654,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6">
         <v>12</v>
       </c>
-      <c r="B6">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
       <c r="D6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -677,22 +677,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
       <c r="D7">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -700,45 +700,45 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>65</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
       <c r="E8">
-        <v>295</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -746,22 +746,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -769,45 +769,45 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>295</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -815,19 +815,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -844,13 +844,13 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -861,22 +861,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>23</v>
@@ -905,10 +905,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="M21" s="1"/>
     </row>
   </sheetData>

</xml_diff>